<commit_message>
pasta trabalho 9 com alteracoes para utilizar OBVs O arquivo foi executado, rodando a RNA 10 vezes e gerou pesos que chegam a marca de 99/100 de acerto
</commit_message>
<xml_diff>
--- a/Trabalho 9/matriz_w.xlsx
+++ b/Trabalho 9/matriz_w.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Study\Engenharia de Computação\Disco virtual\IX Período\Inteligência Artificial\2019_1\Trabalhos\Trabalho 9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{782462AE-B3CF-4730-9ABC-59C20DF7CC4B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{895DAC0E-0D47-4DB0-89D6-52F52D916831}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{FBEEE90D-5DB8-406C-BA3A-CC28BC4ECB04}"/>
   </bookViews>
@@ -371,652 +371,1012 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D6F243-3409-4F7B-92A2-EA7A3EF670CB}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:P20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:J20"/>
+      <selection sqref="A1:P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>0.84926400604510255</v>
+        <v>-0.39471647027722162</v>
       </c>
       <c r="B1">
-        <v>-0.43188577158036606</v>
+        <v>0.65914553784667762</v>
       </c>
       <c r="C1">
-        <v>-0.67427872309387749</v>
+        <v>0.33587960924398585</v>
       </c>
       <c r="D1">
-        <v>-0.73800651873018752</v>
+        <v>1.5518686389190872</v>
       </c>
       <c r="E1">
-        <v>1.2954345357461325</v>
+        <v>-0.72193188720348311</v>
       </c>
       <c r="F1">
-        <v>0.62144359971565122</v>
+        <v>0.40833436122616201</v>
       </c>
       <c r="G1">
-        <v>1.4139735915488654</v>
+        <v>-0.284852230035261</v>
       </c>
       <c r="H1">
-        <v>-1.6635306379216377</v>
+        <v>1.5696061381331852</v>
       </c>
       <c r="I1">
-        <v>0.36192465387134071</v>
+        <v>-0.66643709170887377</v>
       </c>
       <c r="J1">
-        <v>-1.1687017609724413</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-0.17313292082304421</v>
+      </c>
+      <c r="K1">
+        <v>4.7635327332766299E-2</v>
+      </c>
+      <c r="L1">
+        <v>-0.14153863384353801</v>
+      </c>
+      <c r="M1">
+        <v>0.48018766980741356</v>
+      </c>
+      <c r="N1">
+        <v>0.25358450063257548</v>
+      </c>
+      <c r="O1">
+        <v>0.19052256582037005</v>
+      </c>
+      <c r="P1">
+        <v>0.37977328037439029</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>-0.33734100309777543</v>
+        <v>-0.15838749102780716</v>
       </c>
       <c r="B2">
-        <v>1.7117249035867828</v>
+        <v>1.0694314639292821</v>
       </c>
       <c r="C2">
-        <v>-0.10978475107251102</v>
+        <v>-0.86773505377952687</v>
       </c>
       <c r="D2">
-        <v>3.7054656087879653E-2</v>
+        <v>-0.1916733944723851</v>
       </c>
       <c r="E2">
-        <v>0.50947502340846218</v>
+        <v>0.24516304707627573</v>
       </c>
       <c r="F2">
-        <v>0.16838014764334391</v>
+        <v>0.66724758232887393</v>
       </c>
       <c r="G2">
-        <v>0.59261388205154386</v>
+        <v>-1.0834021359068802</v>
       </c>
       <c r="H2">
-        <v>-1.4898772408008842</v>
+        <v>-0.98637239657511688</v>
       </c>
       <c r="I2">
-        <v>-7.3827181065812597E-2</v>
+        <v>-0.62550558538035061</v>
       </c>
       <c r="J2">
-        <v>-1.0884622397225852</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-0.25126068259123369</v>
+      </c>
+      <c r="K2">
+        <v>-1.7949487183131423</v>
+      </c>
+      <c r="L2">
+        <v>-0.85990267961653</v>
+      </c>
+      <c r="M2">
+        <v>-0.90862390787847436</v>
+      </c>
+      <c r="N2">
+        <v>0.7783051172954687</v>
+      </c>
+      <c r="O2">
+        <v>-0.26129919659787781</v>
+      </c>
+      <c r="P2">
+        <v>0.48843610302926699</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2.1268771654605971</v>
+        <v>-0.25194245979209801</v>
       </c>
       <c r="B3">
-        <v>-0.72785926583863081</v>
+        <v>0.92318809889950748</v>
       </c>
       <c r="C3">
-        <v>-0.55946365445648749</v>
+        <v>-1.7537882198181112</v>
       </c>
       <c r="D3">
-        <v>-0.34171801881983754</v>
+        <v>-0.91852362363114026</v>
       </c>
       <c r="E3">
-        <v>1.318357015169255</v>
+        <v>4.766227450196138E-2</v>
       </c>
       <c r="F3">
-        <v>-1.3733455087195243</v>
+        <v>0.93496668430233776</v>
       </c>
       <c r="G3">
-        <v>1.0362839200387219</v>
+        <v>-0.10393081015997996</v>
       </c>
       <c r="H3">
-        <v>-0.76176192394053022</v>
+        <v>4.6130905774274318E-2</v>
       </c>
       <c r="I3">
-        <v>-1.586886290055092</v>
+        <v>-0.31714413490363774</v>
       </c>
       <c r="J3">
-        <v>-0.5681339949391897</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.49990760221048042</v>
+      </c>
+      <c r="K3">
+        <v>1.1300115562892239</v>
+      </c>
+      <c r="L3">
+        <v>1.6662432429930196</v>
+      </c>
+      <c r="M3">
+        <v>1.8392471766565697</v>
+      </c>
+      <c r="N3">
+        <v>2.1400410697047767</v>
+      </c>
+      <c r="O3">
+        <v>-1.2428095057292046</v>
+      </c>
+      <c r="P3">
+        <v>-1.7305014092955771</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>-0.51528461374653589</v>
+        <v>0.37064858323289485</v>
       </c>
       <c r="B4">
-        <v>-0.19000942602906251</v>
+        <v>-1.040062743741633</v>
       </c>
       <c r="C4">
-        <v>-0.41257576907155036</v>
+        <v>1.8291934659492863</v>
       </c>
       <c r="D4">
-        <v>-0.47428519726919288</v>
+        <v>1.5885126550758055</v>
       </c>
       <c r="E4">
-        <v>-0.52994373950530749</v>
+        <v>1.5512687254574344</v>
       </c>
       <c r="F4">
-        <v>0.80919651356312883</v>
+        <v>0.92160204091810971</v>
       </c>
       <c r="G4">
-        <v>0.55699621458017723</v>
+        <v>-1.272578912489595</v>
       </c>
       <c r="H4">
-        <v>0.17784861825448794</v>
+        <v>-2.5100864207717954</v>
       </c>
       <c r="I4">
-        <v>-0.43545008840963639</v>
+        <v>0.91495681455242428</v>
       </c>
       <c r="J4">
-        <v>-1.4165078321873532</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.981749064704647</v>
+      </c>
+      <c r="K4">
+        <v>-2.2857144119709503</v>
+      </c>
+      <c r="L4">
+        <v>-1.7353942146894492</v>
+      </c>
+      <c r="M4">
+        <v>-0.92009729822112252</v>
+      </c>
+      <c r="N4">
+        <v>-0.86599036656872641</v>
+      </c>
+      <c r="O4">
+        <v>1.0583425643762889</v>
+      </c>
+      <c r="P4">
+        <v>1.8596098952750961</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>0.68556130152422268</v>
+        <v>-0.3495845966538913</v>
       </c>
       <c r="B5">
-        <v>1.076029173766005</v>
+        <v>0.73735019722771933</v>
       </c>
       <c r="C5">
-        <v>1.0332669383930682</v>
+        <v>1.0141300353829927</v>
       </c>
       <c r="D5">
-        <v>0.46364772095776163</v>
+        <v>2.733923075053708</v>
       </c>
       <c r="E5">
-        <v>0.37465352504737409</v>
+        <v>1.8398747290340458</v>
       </c>
       <c r="F5">
-        <v>0.7798204387199138</v>
+        <v>2.2127199208226496</v>
       </c>
       <c r="G5">
-        <v>1.3211960993783187</v>
+        <v>-0.27098267241190022</v>
       </c>
       <c r="H5">
-        <v>1.151214674471114</v>
+        <v>0.89162849762886154</v>
       </c>
       <c r="I5">
-        <v>1.1955524343343169</v>
+        <v>-6.0409673263456358E-2</v>
       </c>
       <c r="J5">
-        <v>0.78555236541806561</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-0.39766787726189118</v>
+      </c>
+      <c r="K5">
+        <v>-1.0421838425105543</v>
+      </c>
+      <c r="L5">
+        <v>0.16097523436313529</v>
+      </c>
+      <c r="M5">
+        <v>-0.58585215698362036</v>
+      </c>
+      <c r="N5">
+        <v>-0.86632833511271823</v>
+      </c>
+      <c r="O5">
+        <v>-0.20103964814221298</v>
+      </c>
+      <c r="P5">
+        <v>0.17172768474642475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>-7.1522877139251997E-2</v>
+        <v>-0.69593118044142532</v>
       </c>
       <c r="B6">
-        <v>-0.51740750655097112</v>
+        <v>0.68434527645856247</v>
       </c>
       <c r="C6">
-        <v>-1.8883051476502954</v>
+        <v>1.5554454669375835</v>
       </c>
       <c r="D6">
-        <v>-0.37309192320663215</v>
+        <v>2.0253632396565857</v>
       </c>
       <c r="E6">
-        <v>0.28606129375760692</v>
+        <v>-1.6131505953445695</v>
       </c>
       <c r="F6">
-        <v>0.26273138560921455</v>
+        <v>-0.65012357107814067</v>
       </c>
       <c r="G6">
-        <v>5.7918557737253545E-2</v>
+        <v>-2.1547897618430119</v>
       </c>
       <c r="H6">
-        <v>1.2393285191527634</v>
+        <v>-1.5300742660739328</v>
       </c>
       <c r="I6">
-        <v>-0.35147529831028507</v>
+        <v>1.3859886129611374</v>
       </c>
       <c r="J6">
-        <v>7.3662239600980964E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.3036023862078219</v>
+      </c>
+      <c r="K6">
+        <v>2.0586389215983485</v>
+      </c>
+      <c r="L6">
+        <v>2.5703271466206692</v>
+      </c>
+      <c r="M6">
+        <v>-0.97256222262263659</v>
+      </c>
+      <c r="N6">
+        <v>-0.6505030734174766</v>
+      </c>
+      <c r="O6">
+        <v>-0.82428277488987967</v>
+      </c>
+      <c r="P6">
+        <v>-1.375364631356683</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>0.15182486291195013</v>
+        <v>0.18142673761292841</v>
       </c>
       <c r="B7">
-        <v>0.54068240666615075</v>
+        <v>-0.50332661434509052</v>
       </c>
       <c r="C7">
-        <v>-0.2364122806457668</v>
+        <v>1.2677953915364466</v>
       </c>
       <c r="D7">
-        <v>0.66486794572150032</v>
+        <v>0.51886852667218208</v>
       </c>
       <c r="E7">
-        <v>-0.14642549441218888</v>
+        <v>1.5866187366035649</v>
       </c>
       <c r="F7">
-        <v>-0.91768696972618735</v>
+        <v>0.59205963064410183</v>
       </c>
       <c r="G7">
-        <v>0.27308323300866821</v>
+        <v>0.91640684448844267</v>
       </c>
       <c r="H7">
-        <v>-0.54671515087356881</v>
+        <v>0.47788280246435622</v>
       </c>
       <c r="I7">
-        <v>4.4543321798132411E-2</v>
+        <v>-0.82631942696863747</v>
       </c>
       <c r="J7">
-        <v>-0.32534867405336265</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.6938432982563181</v>
+      </c>
+      <c r="K7">
+        <v>-1.4813752850257444</v>
+      </c>
+      <c r="L7">
+        <v>1.1660246224492656</v>
+      </c>
+      <c r="M7">
+        <v>-2.1963209637776462</v>
+      </c>
+      <c r="N7">
+        <v>-0.16259928850084326</v>
+      </c>
+      <c r="O7">
+        <v>-2.1175028181722171</v>
+      </c>
+      <c r="P7">
+        <v>3.5197444588572671E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>-1.4401403010175517</v>
+        <v>-0.20759465107050717</v>
       </c>
       <c r="B8">
-        <v>-0.17920655350297865</v>
+        <v>0.9786681281695947</v>
       </c>
       <c r="C8">
-        <v>-0.60510589014134708</v>
+        <v>1.3597210320427644</v>
       </c>
       <c r="D8">
-        <v>0.42454645811527836</v>
+        <v>1.5394047842123557</v>
       </c>
       <c r="E8">
-        <v>1.3445203197176385</v>
+        <v>2.227731681737374</v>
       </c>
       <c r="F8">
-        <v>2.035446149482051</v>
+        <v>0.74253183932702493</v>
       </c>
       <c r="G8">
-        <v>1.2010368949348003</v>
+        <v>-0.60058768512976302</v>
       </c>
       <c r="H8">
-        <v>0.30789284661851057</v>
+        <v>-4.0844124920266241E-2</v>
       </c>
       <c r="I8">
-        <v>-1.480155908256181</v>
+        <v>1.2518715894650605</v>
       </c>
       <c r="J8">
-        <v>-1.7996951826772167</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.60612749954603484</v>
+      </c>
+      <c r="K8">
+        <v>-0.97262133054673683</v>
+      </c>
+      <c r="L8">
+        <v>-1.8818484234264365</v>
+      </c>
+      <c r="M8">
+        <v>0.82584817858690152</v>
+      </c>
+      <c r="N8">
+        <v>6.3487276285363728E-2</v>
+      </c>
+      <c r="O8">
+        <v>6.1035419665688241E-2</v>
+      </c>
+      <c r="P8">
+        <v>-0.67698547954716337</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>-0.88351331094561492</v>
+        <v>0.15637258285957609</v>
       </c>
       <c r="B9">
-        <v>-0.86021342370229459</v>
+        <v>2.0253089611719179</v>
       </c>
       <c r="C9">
-        <v>-2.7701497239064336E-2</v>
+        <v>-0.16616221461966582</v>
       </c>
       <c r="D9">
-        <v>-1.3327738828430671</v>
+        <v>2.0317426799641578</v>
       </c>
       <c r="E9">
-        <v>0.37251419730753221</v>
+        <v>-1.0975413125117437</v>
       </c>
       <c r="F9">
-        <v>-0.66211810452650566</v>
+        <v>0.84343539041634474</v>
       </c>
       <c r="G9">
-        <v>0.83940990326319931</v>
+        <v>-1.2985331137580651</v>
       </c>
       <c r="H9">
-        <v>0.63405776328519969</v>
+        <v>1.6961270383812632</v>
       </c>
       <c r="I9">
-        <v>1.6696159931265662</v>
+        <v>0.36749443781527086</v>
       </c>
       <c r="J9">
-        <v>-1.158920548455505</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.73277661185835263</v>
+      </c>
+      <c r="K9">
+        <v>1.400292314654735</v>
+      </c>
+      <c r="L9">
+        <v>1.7725891269178427</v>
+      </c>
+      <c r="M9">
+        <v>-2.5135246772912367</v>
+      </c>
+      <c r="N9">
+        <v>-0.95709758379067511</v>
+      </c>
+      <c r="O9">
+        <v>-0.75270305439452423</v>
+      </c>
+      <c r="P9">
+        <v>-0.13396814553772438</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1.1043647500722933</v>
+        <v>0.20217726297184119</v>
       </c>
       <c r="B10">
-        <v>0.69256350673086342</v>
+        <v>-0.63915705571942916</v>
       </c>
       <c r="C10">
-        <v>1.0500647506455365</v>
+        <v>-0.47542822916255784</v>
       </c>
       <c r="D10">
-        <v>1.3278157686610517</v>
+        <v>-1.3066198379806324</v>
       </c>
       <c r="E10">
-        <v>0.14230201238170564</v>
+        <v>0.73267567418624924</v>
       </c>
       <c r="F10">
-        <v>0.54435927664263561</v>
+        <v>0.29004547645302881</v>
       </c>
       <c r="G10">
-        <v>0.71108192289140737</v>
+        <v>-0.50197105466344072</v>
       </c>
       <c r="H10">
-        <v>0.52069869595039364</v>
+        <v>-1.6598277688361083</v>
       </c>
       <c r="I10">
-        <v>0.77790146644207936</v>
+        <v>1.5205281451855592</v>
       </c>
       <c r="J10">
-        <v>-0.1228379861805944</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.23478883109019222</v>
+      </c>
+      <c r="K10">
+        <v>1.4054311200079461</v>
+      </c>
+      <c r="L10">
+        <v>-0.44245426847375602</v>
+      </c>
+      <c r="M10">
+        <v>0.58444065257861266</v>
+      </c>
+      <c r="N10">
+        <v>-1.3493943401251292</v>
+      </c>
+      <c r="O10">
+        <v>0.46606873501357921</v>
+      </c>
+      <c r="P10">
+        <v>-0.48775726666255131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0.56033198176619059</v>
+        <v>-0.8133700949433752</v>
       </c>
       <c r="B11">
-        <v>-0.75981359405106719</v>
+        <v>4.8301447151299408E-2</v>
       </c>
       <c r="C11">
-        <v>1.1011248747362909</v>
+        <v>-2.0387169037937118</v>
       </c>
       <c r="D11">
-        <v>2.097596947779532</v>
+        <v>-1.7038291846177058</v>
       </c>
       <c r="E11">
-        <v>-0.64045896420628967</v>
+        <v>-4.3088761728007405</v>
       </c>
       <c r="F11">
-        <v>-0.96879280178765237</v>
+        <v>-3.8906450849857848</v>
       </c>
       <c r="G11">
-        <v>0.30631089482077301</v>
+        <v>3.1843409335218356</v>
       </c>
       <c r="H11">
-        <v>1.3850127725876118</v>
+        <v>2.9819175097573822</v>
       </c>
       <c r="I11">
-        <v>-0.49770973718897554</v>
+        <v>0.54680323746063353</v>
       </c>
       <c r="J11">
-        <v>-1.546641042367537</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.0067177942142158</v>
+      </c>
+      <c r="K11">
+        <v>-3.2523853790153647</v>
+      </c>
+      <c r="L11">
+        <v>-2.7906708459793017</v>
+      </c>
+      <c r="M11">
+        <v>-3.3571943151662138</v>
+      </c>
+      <c r="N11">
+        <v>-2.644285039520339</v>
+      </c>
+      <c r="O11">
+        <v>2.3486413258967462</v>
+      </c>
+      <c r="P11">
+        <v>3.2714773470059781</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>0.24947825162460255</v>
+        <v>-0.41774785844323181</v>
       </c>
       <c r="B12">
-        <v>0.40160518621070923</v>
+        <v>-1.8623386789802037</v>
       </c>
       <c r="C12">
-        <v>0.84736556066569724</v>
+        <v>0.94283188094939474</v>
       </c>
       <c r="D12">
-        <v>0.26837227306036754</v>
+        <v>-2.5189004825346282</v>
       </c>
       <c r="E12">
-        <v>0.37925942536923729</v>
+        <v>0.32441648336346962</v>
       </c>
       <c r="F12">
-        <v>7.0123812669439317E-2</v>
+        <v>-2.630802885972761</v>
       </c>
       <c r="G12">
-        <v>0.6580816976886793</v>
+        <v>1.7762606538993795</v>
       </c>
       <c r="H12">
-        <v>0.32841132263153555</v>
+        <v>-1.536337412987113</v>
       </c>
       <c r="I12">
-        <v>-0.48402063339019036</v>
+        <v>-1.6235506228571581</v>
       </c>
       <c r="J12">
-        <v>-0.99774947721873652</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+        <v>3.5492042247673852</v>
+      </c>
+      <c r="K12">
+        <v>-1.6303254085576988</v>
+      </c>
+      <c r="L12">
+        <v>2.8396253306772326</v>
+      </c>
+      <c r="M12">
+        <v>-3.0286474522149516</v>
+      </c>
+      <c r="N12">
+        <v>1.2339837248164767</v>
+      </c>
+      <c r="O12">
+        <v>-4.5327240638241806</v>
+      </c>
+      <c r="P12">
+        <v>2.287924670451845</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>0.11953383977034397</v>
+        <v>0.36744870925516532</v>
       </c>
       <c r="B13">
-        <v>-0.74953666380895256</v>
+        <v>0.56842398281002482</v>
       </c>
       <c r="C13">
-        <v>-2.2403739943431988</v>
+        <v>-1.0389372641823766</v>
       </c>
       <c r="D13">
-        <v>2.3225426667823612</v>
+        <v>-0.23553684475389317</v>
       </c>
       <c r="E13">
-        <v>0.12207385454009047</v>
+        <v>-1.3575023451134345</v>
       </c>
       <c r="F13">
-        <v>1.0881897784309036</v>
+        <v>-1.3872783311595889</v>
       </c>
       <c r="G13">
-        <v>-4.7159633630360645E-2</v>
+        <v>-1.6988903556814001</v>
       </c>
       <c r="H13">
-        <v>-1.4471073742887031</v>
+        <v>-1.3722718154610967</v>
       </c>
       <c r="I13">
-        <v>0.1362410309555403</v>
+        <v>-9.6202760261499098E-2</v>
       </c>
       <c r="J13">
-        <v>0.82028776985229923</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.9233155083990487</v>
+      </c>
+      <c r="K13">
+        <v>0.19650568280113781</v>
+      </c>
+      <c r="L13">
+        <v>3.3182083037346906</v>
+      </c>
+      <c r="M13">
+        <v>8.0525109064931544E-2</v>
+      </c>
+      <c r="N13">
+        <v>2.4478999709580278</v>
+      </c>
+      <c r="O13">
+        <v>-0.65225420613658069</v>
+      </c>
+      <c r="P13">
+        <v>1.3026547778794912</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>0.82198449052139133</v>
+        <v>0.39047273811867955</v>
       </c>
       <c r="B14">
-        <v>-1.3146427003734371</v>
+        <v>2.6421376524114506</v>
       </c>
       <c r="C14">
-        <v>0.58555822789983181</v>
+        <v>-0.58752267695183402</v>
       </c>
       <c r="D14">
-        <v>-0.97736746155904963</v>
+        <v>1.2996070487474611</v>
       </c>
       <c r="E14">
-        <v>-1.3186323262088695</v>
+        <v>-1.2890444373719432</v>
       </c>
       <c r="F14">
-        <v>1.2725196025969077</v>
+        <v>0.27494339063869455</v>
       </c>
       <c r="G14">
-        <v>-0.46170966739141256</v>
+        <v>-1.0013618000829279</v>
       </c>
       <c r="H14">
-        <v>-0.82714121798809814</v>
+        <v>0.84485177012453261</v>
       </c>
       <c r="I14">
-        <v>-1.6457194471615133</v>
+        <v>-0.78238116005712655</v>
       </c>
       <c r="J14">
-        <v>1.179989142057889</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+        <v>2.435482622740357</v>
+      </c>
+      <c r="K14">
+        <v>-2.5423875255707826</v>
+      </c>
+      <c r="L14">
+        <v>1.6738389777009111</v>
+      </c>
+      <c r="M14">
+        <v>-2.1003195548381255</v>
+      </c>
+      <c r="N14">
+        <v>1.801820613966252</v>
+      </c>
+      <c r="O14">
+        <v>-2.7623412724190777</v>
+      </c>
+      <c r="P14">
+        <v>2.2922720436914177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>0.16421589602942505</v>
+        <v>0.19886483798400229</v>
       </c>
       <c r="B15">
-        <v>-0.1618288440432244</v>
+        <v>-1.5226213630272567</v>
       </c>
       <c r="C15">
-        <v>0.58147767448300769</v>
+        <v>1.2418464506511351</v>
       </c>
       <c r="D15">
-        <v>0.25380820450458386</v>
+        <v>0.74551764461948999</v>
       </c>
       <c r="E15">
-        <v>-2.4542823684945669</v>
+        <v>-1.5873634243149424</v>
       </c>
       <c r="F15">
-        <v>0.83556718595706114</v>
+        <v>-1.620427763544465</v>
       </c>
       <c r="G15">
-        <v>2.5443056703282934</v>
+        <v>0.25409724053301003</v>
       </c>
       <c r="H15">
-        <v>-0.7363984609783889</v>
+        <v>-0.29119787869112207</v>
       </c>
       <c r="I15">
-        <v>0.75860259406773733</v>
+        <v>1.382357720320504</v>
       </c>
       <c r="J15">
-        <v>-5.7258381790881975E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1.5077365475306812</v>
+      </c>
+      <c r="K15">
+        <v>-0.98545247292116533</v>
+      </c>
+      <c r="L15">
+        <v>-1.3524120120472349</v>
+      </c>
+      <c r="M15">
+        <v>1.6212708137731018</v>
+      </c>
+      <c r="N15">
+        <v>1.1642008221525868</v>
+      </c>
+      <c r="O15">
+        <v>-2.1495504340686353</v>
+      </c>
+      <c r="P15">
+        <v>-1.6156822332979839</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>-0.58746142289539549</v>
+        <v>-0.18788140687135693</v>
       </c>
       <c r="B16">
-        <v>-1.3847116748979749</v>
+        <v>0.79972226532244672</v>
       </c>
       <c r="C16">
-        <v>-1.2609955229886634</v>
+        <v>1.2853952718687132</v>
       </c>
       <c r="D16">
-        <v>-1.3722253264548994</v>
+        <v>1.2814743437100069</v>
       </c>
       <c r="E16">
-        <v>-1.0624603024483952</v>
+        <v>-1.161820620162993</v>
       </c>
       <c r="F16">
-        <v>-1.353773691483547</v>
+        <v>-1.4911228715619593</v>
       </c>
       <c r="G16">
-        <v>-0.77514640510035493</v>
+        <v>-1.5281749817677548</v>
       </c>
       <c r="H16">
-        <v>-1.66619705298764</v>
+        <v>-2.9543221122268699</v>
       </c>
       <c r="I16">
-        <v>-0.64595393873047857</v>
+        <v>1.566871477923985</v>
       </c>
       <c r="J16">
-        <v>-0.29410764347419988</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.65989495529715869</v>
+      </c>
+      <c r="K16">
+        <v>0.16590119679796977</v>
+      </c>
+      <c r="L16">
+        <v>-0.72360176586360914</v>
+      </c>
+      <c r="M16">
+        <v>0.62166832706761999</v>
+      </c>
+      <c r="N16">
+        <v>3.4368028916248856E-2</v>
+      </c>
+      <c r="O16">
+        <v>0.1520860978115659</v>
+      </c>
+      <c r="P16">
+        <v>-0.12524417146398939</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>-0.51295225773893716</v>
+        <v>-9.1379341418448945E-2</v>
       </c>
       <c r="B17">
-        <v>-0.54934623279620454</v>
+        <v>-0.95739065456981598</v>
       </c>
       <c r="C17">
-        <v>-0.88151259030729301</v>
+        <v>0.82112481688357963</v>
       </c>
       <c r="D17">
-        <v>-1.2940858311592025</v>
+        <v>0.52260602326022432</v>
       </c>
       <c r="E17">
-        <v>-0.92075229889744359</v>
+        <v>1.0257886874207562</v>
       </c>
       <c r="F17">
-        <v>-0.62939593697908214</v>
+        <v>0.84858217200160135</v>
       </c>
       <c r="G17">
-        <v>-1.1216013470050361</v>
+        <v>-1.7631246422616862</v>
       </c>
       <c r="H17">
-        <v>-0.64017900444208664</v>
+        <v>-1.1081620199976452</v>
       </c>
       <c r="I17">
-        <v>-0.39753485034396641</v>
+        <v>-2.1034338239625936</v>
       </c>
       <c r="J17">
-        <v>-1.06689203548889</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-3.0069973971410349</v>
+      </c>
+      <c r="K17">
+        <v>1.9773378949944889</v>
+      </c>
+      <c r="L17">
+        <v>1.3052690792202108</v>
+      </c>
+      <c r="M17">
+        <v>-2.1361965320291181</v>
+      </c>
+      <c r="N17">
+        <v>-2.6367128646834397</v>
+      </c>
+      <c r="O17">
+        <v>-0.72130289409828396</v>
+      </c>
+      <c r="P17">
+        <v>-2.2605406043904006</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>-0.52471496385358596</v>
+        <v>0.12713157742068174</v>
       </c>
       <c r="B18">
-        <v>1.3346916491113485</v>
+        <v>0.9450174414418161</v>
       </c>
       <c r="C18">
-        <v>1.4461718408686659</v>
+        <v>1.7980413812728855</v>
       </c>
       <c r="D18">
-        <v>0.26840922665611633</v>
+        <v>2.4335794037618688</v>
       </c>
       <c r="E18">
-        <v>-0.39677365838215334</v>
+        <v>-0.79355599946173949</v>
       </c>
       <c r="F18">
-        <v>0.3746195085118289</v>
+        <v>-1.1612782622807949</v>
       </c>
       <c r="G18">
-        <v>0.6765895813435242</v>
+        <v>3.8558219731949244</v>
       </c>
       <c r="H18">
-        <v>0.13348932619768419</v>
+        <v>2.3464584421511612</v>
       </c>
       <c r="I18">
-        <v>-1.1826963230691279</v>
+        <v>-2.10434607048294</v>
       </c>
       <c r="J18">
-        <v>-1.1989325249875344</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+        <v>-2.2739219978818732</v>
+      </c>
+      <c r="K18">
+        <v>1.6770655494658873</v>
+      </c>
+      <c r="L18">
+        <v>1.7056719269738343</v>
+      </c>
+      <c r="M18">
+        <v>-0.8720205212922939</v>
+      </c>
+      <c r="N18">
+        <v>-1.6547517323320868</v>
+      </c>
+      <c r="O18">
+        <v>1.4847611903328433</v>
+      </c>
+      <c r="P18">
+        <v>1.5690376907488457</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>0.50767801694568671</v>
+        <v>9.8525226442088332E-2</v>
       </c>
       <c r="B19">
-        <v>0.58300349791804962</v>
+        <v>2.2269596896528818</v>
       </c>
       <c r="C19">
-        <v>1.0403969810696843</v>
+        <v>-1.478934678639491</v>
       </c>
       <c r="D19">
-        <v>0.20304313596864609</v>
+        <v>-0.59886764954040383</v>
       </c>
       <c r="E19">
-        <v>0.17867786610760303</v>
+        <v>-0.99611901094633581</v>
       </c>
       <c r="F19">
-        <v>1.4471681951483382</v>
+        <v>9.4983666758980248E-2</v>
       </c>
       <c r="G19">
-        <v>0.77104630030937005</v>
+        <v>-7.1545560552431997E-2</v>
       </c>
       <c r="H19">
-        <v>1.5958244276384064</v>
+        <v>0.58076003366246476</v>
       </c>
       <c r="I19">
-        <v>0.70166456033771307</v>
+        <v>1.1674027273320429</v>
       </c>
       <c r="J19">
-        <v>1.3889226230059051</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+        <v>0.36681760366601424</v>
+      </c>
+      <c r="K19">
+        <v>0.12207579679128623</v>
+      </c>
+      <c r="L19">
+        <v>-0.52351986980581955</v>
+      </c>
+      <c r="M19">
+        <v>-0.35843593080447206</v>
+      </c>
+      <c r="N19">
+        <v>-1.1540322349283101</v>
+      </c>
+      <c r="O19">
+        <v>-1.5543826065493576</v>
+      </c>
+      <c r="P19">
+        <v>-1.1995466528193688</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>-0.92454441277901367</v>
+        <v>-0.17491602529818881</v>
       </c>
       <c r="B20">
-        <v>1.5048718181026319</v>
+        <v>-1.8201543407622165</v>
       </c>
       <c r="C20">
-        <v>-1.4236906105915246</v>
+        <v>2.4481782185588674</v>
       </c>
       <c r="D20">
-        <v>0.91440022465267301</v>
+        <v>-0.98537596063169053</v>
       </c>
       <c r="E20">
-        <v>0.18509059616274415</v>
+        <v>1.0651986237946807</v>
       </c>
       <c r="F20">
-        <v>-0.94046680898697788</v>
+        <v>-0.98735694314341005</v>
       </c>
       <c r="G20">
-        <v>-0.56271766858148131</v>
+        <v>1.275759038688183</v>
       </c>
       <c r="H20">
-        <v>1.1477155121146596</v>
+        <v>-7.8515453794665679E-2</v>
       </c>
       <c r="I20">
-        <v>-1.3275749535453609</v>
+        <v>1.4698609919289827</v>
       </c>
       <c r="J20">
-        <v>0.34640247366135779</v>
+        <v>0.15686540533342455</v>
+      </c>
+      <c r="K20">
+        <v>0.9609312525777296</v>
+      </c>
+      <c r="L20">
+        <v>1.0292430100398452E-2</v>
+      </c>
+      <c r="M20">
+        <v>1.5896566323996018</v>
+      </c>
+      <c r="N20">
+        <v>1.2074678908964933</v>
+      </c>
+      <c r="O20">
+        <v>0.6198894222870498</v>
+      </c>
+      <c r="P20">
+        <v>0.2443936543559212</v>
       </c>
     </row>
   </sheetData>

</xml_diff>